<commit_message>
Documentation Updates for Release
Documentation updates for March 12, 2018 Release (v18.312)
</commit_message>
<xml_diff>
--- a/Docs/Sample Data - Interactions for Student Recruitment.xlsx
+++ b/Docs/Sample Data - Interactions for Student Recruitment.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\missk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nina.gomez\Box Sync\Force For Change Project - 2018\LIVE AND PUBLISHED\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12930" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Interaction Mappings" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="276">
   <si>
     <t>NAME</t>
   </si>
@@ -670,9 +670,6 @@
     <t>Skip Mapping</t>
   </si>
   <si>
-    <t>Interaction Source Field API Name</t>
-  </si>
-  <si>
     <t>Target Field API Name</t>
   </si>
   <si>
@@ -851,12 +848,21 @@
   </si>
   <si>
     <t>Admitted</t>
+  </si>
+  <si>
+    <t>Source Field API Name</t>
+  </si>
+  <si>
+    <t>Source Object API Name</t>
+  </si>
+  <si>
+    <t>Interaction__c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1722,24 +1728,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.3984375" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>210</v>
       </c>
@@ -1750,16 +1756,19 @@
         <v>212</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G1" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="b">
         <v>1</v>
       </c>
@@ -1776,8 +1785,11 @@
       <c r="F2" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="b">
         <v>1</v>
       </c>
@@ -1794,8 +1806,11 @@
       <c r="F3" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G3" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="b">
         <v>1</v>
       </c>
@@ -1812,8 +1827,11 @@
       <c r="F4" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G4" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="b">
         <v>1</v>
       </c>
@@ -1830,8 +1848,11 @@
       <c r="F5" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G5" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="b">
         <v>1</v>
       </c>
@@ -1848,8 +1869,11 @@
       <c r="F6" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G6" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="b">
         <v>1</v>
       </c>
@@ -1866,8 +1890,11 @@
       <c r="F7" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G7" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="b">
         <v>1</v>
       </c>
@@ -1884,8 +1911,11 @@
       <c r="F8" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G8" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="b">
         <v>1</v>
       </c>
@@ -1902,8 +1932,11 @@
       <c r="F9" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G9" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="b">
         <v>1</v>
       </c>
@@ -1920,8 +1953,11 @@
       <c r="F10" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G10" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="b">
         <v>1</v>
       </c>
@@ -1938,8 +1974,11 @@
       <c r="F11" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G11" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="b">
         <v>1</v>
       </c>
@@ -1956,8 +1995,11 @@
       <c r="F12" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G12" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="b">
         <v>1</v>
       </c>
@@ -1974,8 +2016,11 @@
       <c r="F13" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G13" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="b">
         <v>1</v>
       </c>
@@ -1992,8 +2037,11 @@
       <c r="F14" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G14" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="b">
         <v>1</v>
       </c>
@@ -2010,8 +2058,11 @@
       <c r="F15" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G15" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="b">
         <v>1</v>
       </c>
@@ -2028,8 +2079,11 @@
       <c r="F16" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G16" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="b">
         <v>1</v>
       </c>
@@ -2046,8 +2100,11 @@
       <c r="F17" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G17" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="b">
         <v>1</v>
       </c>
@@ -2064,8 +2121,11 @@
       <c r="F18" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G18" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="b">
         <v>1</v>
       </c>
@@ -2082,8 +2142,11 @@
       <c r="F19" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G19" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="b">
         <v>1</v>
       </c>
@@ -2100,8 +2163,11 @@
       <c r="F20" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G20" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="b">
         <v>1</v>
       </c>
@@ -2118,8 +2184,11 @@
       <c r="F21" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G21" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="b">
         <v>1</v>
       </c>
@@ -2136,8 +2205,11 @@
       <c r="F22" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G22" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="b">
         <v>1</v>
       </c>
@@ -2154,8 +2226,11 @@
       <c r="F23" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G23" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="b">
         <v>1</v>
       </c>
@@ -2172,8 +2247,11 @@
       <c r="F24" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G24" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="b">
         <v>1</v>
       </c>
@@ -2190,8 +2268,11 @@
       <c r="F25" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G25" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="b">
         <v>1</v>
       </c>
@@ -2208,8 +2289,11 @@
       <c r="F26" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G26" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="b">
         <v>1</v>
       </c>
@@ -2226,8 +2310,11 @@
       <c r="F27" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G27" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="b">
         <v>1</v>
       </c>
@@ -2244,8 +2331,11 @@
       <c r="F28" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G28" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="b">
         <v>1</v>
       </c>
@@ -2262,8 +2352,11 @@
       <c r="F29" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G29" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="b">
         <v>1</v>
       </c>
@@ -2280,8 +2373,11 @@
       <c r="F30" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G30" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="b">
         <v>1</v>
       </c>
@@ -2298,8 +2394,11 @@
       <c r="F31" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G31" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="b">
         <v>1</v>
       </c>
@@ -2316,8 +2415,11 @@
       <c r="F32" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G32" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="b">
         <v>1</v>
       </c>
@@ -2334,8 +2436,11 @@
       <c r="F33" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G33" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="b">
         <v>1</v>
       </c>
@@ -2352,8 +2457,11 @@
       <c r="F34" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G34" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="b">
         <v>1</v>
       </c>
@@ -2370,8 +2478,11 @@
       <c r="F35" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G35" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="b">
         <v>1</v>
       </c>
@@ -2388,8 +2499,11 @@
       <c r="F36" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G36" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="b">
         <v>1</v>
       </c>
@@ -2406,8 +2520,11 @@
       <c r="F37" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G37" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="b">
         <v>1</v>
       </c>
@@ -2424,8 +2541,11 @@
       <c r="F38" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G38" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="b">
         <v>1</v>
       </c>
@@ -2442,8 +2562,11 @@
       <c r="F39" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G39" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="b">
         <v>1</v>
       </c>
@@ -2460,8 +2583,11 @@
       <c r="F40" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G40" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="b">
         <v>1</v>
       </c>
@@ -2478,8 +2604,11 @@
       <c r="F41" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G41" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="b">
         <v>1</v>
       </c>
@@ -2496,8 +2625,11 @@
       <c r="F42" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G42" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="b">
         <v>1</v>
       </c>
@@ -2514,8 +2646,11 @@
       <c r="F43" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G43" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="b">
         <v>1</v>
       </c>
@@ -2532,8 +2667,11 @@
       <c r="F44" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G44" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="b">
         <v>1</v>
       </c>
@@ -2550,8 +2688,11 @@
       <c r="F45" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G45" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="b">
         <v>1</v>
       </c>
@@ -2560,16 +2701,19 @@
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G46" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="b">
         <v>1</v>
       </c>
@@ -2586,8 +2730,11 @@
       <c r="F47" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G47" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="b">
         <v>1</v>
       </c>
@@ -2604,8 +2751,11 @@
       <c r="F48" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G48" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="b">
         <v>1</v>
       </c>
@@ -2622,8 +2772,11 @@
       <c r="F49" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G49" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="b">
         <v>1</v>
       </c>
@@ -2640,8 +2793,11 @@
       <c r="F50" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G50" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="b">
         <v>1</v>
       </c>
@@ -2658,8 +2814,11 @@
       <c r="F51" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G51" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="b">
         <v>1</v>
       </c>
@@ -2676,8 +2835,11 @@
       <c r="F52" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G52" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="b">
         <v>1</v>
       </c>
@@ -2694,8 +2856,11 @@
       <c r="F53" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G53" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="b">
         <v>1</v>
       </c>
@@ -2712,8 +2877,11 @@
       <c r="F54" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G54" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="b">
         <v>1</v>
       </c>
@@ -2722,16 +2890,19 @@
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G55" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="b">
         <v>1</v>
       </c>
@@ -2748,8 +2919,11 @@
       <c r="F56" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G56" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="b">
         <v>1</v>
       </c>
@@ -2766,8 +2940,11 @@
       <c r="F57" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G57" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="b">
         <v>1</v>
       </c>
@@ -2784,8 +2961,11 @@
       <c r="F58" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G58" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="b">
         <v>1</v>
       </c>
@@ -2802,8 +2982,11 @@
       <c r="F59" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G59" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="b">
         <v>1</v>
       </c>
@@ -2820,8 +3003,11 @@
       <c r="F60" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G60" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="b">
         <v>1</v>
       </c>
@@ -2838,8 +3024,11 @@
       <c r="F61" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G61" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="b">
         <v>1</v>
       </c>
@@ -2848,16 +3037,19 @@
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G62" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="b">
         <v>1</v>
       </c>
@@ -2874,8 +3066,11 @@
       <c r="F63" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G63" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -2890,27 +3085,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2939,7 +3134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2965,9 +3160,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -2988,10 +3183,10 @@
         <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3017,7 +3212,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3043,7 +3238,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3069,7 +3264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3097,37 +3292,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" display="http://www.astrou.edu" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2" display="http://www.astrou.edu"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3135,7 +3330,7 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
@@ -3147,10 +3342,10 @@
         <v>52</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -3170,10 +3365,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -3193,10 +3388,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3216,10 +3411,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -3239,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3248,42 +3443,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F1" t="s">
         <v>50</v>
@@ -3295,10 +3490,10 @@
         <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3324,11 +3519,11 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -3354,11 +3549,11 @@
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -3384,11 +3579,11 @@
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -3414,11 +3609,11 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -3444,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J6" s="6"/>
     </row>
@@ -3454,22 +3649,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3483,12 +3678,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" s="2">
         <v>43101</v>
@@ -3497,12 +3692,12 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="2">
         <v>43221</v>
@@ -3511,12 +3706,12 @@
         <v>43343</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" s="2">
         <v>43344</v>
@@ -3525,12 +3720,12 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" s="2">
         <v>43466</v>
@@ -3539,12 +3734,12 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="2">
         <v>43586</v>
@@ -3553,12 +3748,12 @@
         <v>43708</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C7" s="2">
         <v>43709</v>
@@ -3574,23 +3769,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3610,7 +3805,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>194</v>
       </c>
@@ -3630,7 +3825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>198</v>
       </c>
@@ -3650,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>199</v>
       </c>
@@ -3676,77 +3871,77 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.1328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.3984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>92</v>
@@ -3758,19 +3953,19 @@
         <v>93</v>
       </c>
       <c r="P1" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q1" t="s">
         <v>227</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S1" t="s">
+        <v>267</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="R1" t="s">
-        <v>263</v>
-      </c>
-      <c r="S1" t="s">
-        <v>268</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>76</v>
@@ -3785,9 +3980,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>28</v>
@@ -3859,7 +4054,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
@@ -3888,7 +4083,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>41</v>
@@ -3906,7 +4101,7 @@
         <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q3" t="s">
         <v>74</v>
@@ -3933,12 +4128,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>44</v>
@@ -3978,7 +4173,7 @@
         <v>48</v>
       </c>
       <c r="P4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>74</v>
@@ -4000,15 +4195,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>12</v>
@@ -4023,13 +4218,13 @@
         <v>14</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="L5" s="2">
         <v>36600</v>
@@ -4041,7 +4236,7 @@
         <v>42</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>118</v>
@@ -4071,15 +4266,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>12</v>
@@ -4094,10 +4289,10 @@
         <v>14</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>41</v>
@@ -4115,7 +4310,7 @@
         <v>208</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>73</v>
@@ -4142,15 +4337,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>12</v>
@@ -4165,13 +4360,13 @@
         <v>14</v>
       </c>
       <c r="H7" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="K7" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L7" s="2">
         <v>35100</v>
@@ -4198,7 +4393,7 @@
         <v>199</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V7" s="6" t="b">
         <v>1</v>
@@ -4210,15 +4405,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
         <v>249</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>250</v>
-      </c>
-      <c r="C8" t="s">
-        <v>251</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -4233,10 +4428,10 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J8" t="s">
         <v>252</v>
-      </c>
-      <c r="J8" t="s">
-        <v>253</v>
       </c>
       <c r="K8" t="s">
         <v>41</v>
@@ -4264,7 +4459,7 @@
         <v>199</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V8" s="6" t="b">
         <v>1</v>
@@ -4276,15 +4471,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" t="s">
         <v>256</v>
-      </c>
-      <c r="B9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" t="s">
-        <v>257</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -4299,10 +4494,10 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" t="s">
         <v>258</v>
-      </c>
-      <c r="J9" t="s">
-        <v>259</v>
       </c>
       <c r="K9" t="s">
         <v>33</v>
@@ -4317,7 +4512,7 @@
         <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P9" t="s">
         <v>118</v>
@@ -4354,37 +4549,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4440,10 +4635,10 @@
         <v>94</v>
       </c>
       <c r="S1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -4499,7 +4694,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>202</v>
       </c>

</xml_diff>